<commit_message>
Targets concentrations in QCs added to the file
</commit_message>
<xml_diff>
--- a/results/Melanie_new_suspects/310523_DataForFigures.xlsx
+++ b/results/Melanie_new_suspects/310523_DataForFigures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MelanieLauria\Documents\GitHub\PFOA_semi_quant\results\Melanie_new_suspects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E98BCD-CDA0-41A1-B1EA-34C2B9E6604E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AABFAB-75EA-4C2C-B046-7B97D28C6E1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="5475" activeTab="4" xr2:uid="{9AAFE6A4-0CE6-4820-A6A0-22E494B0EACC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15468" windowHeight="5472" activeTab="1" xr2:uid="{9AAFE6A4-0CE6-4820-A6A0-22E494B0EACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="66">
   <si>
     <t>PFPeA</t>
   </si>
@@ -136,18 +136,6 @@
     <t>11Cl-PF3OUdS</t>
   </si>
   <si>
-    <t>Compounds</t>
-  </si>
-  <si>
-    <t>QC_A</t>
-  </si>
-  <si>
-    <t>QC_B</t>
-  </si>
-  <si>
-    <t>QC_C</t>
-  </si>
-  <si>
     <t>Sample</t>
   </si>
   <si>
@@ -231,6 +219,18 @@
   <si>
     <t>∑Suspects</t>
   </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>QCN-AL</t>
+  </si>
+  <si>
+    <t>QCN-BL</t>
+  </si>
+  <si>
+    <t>QCN-CL</t>
+  </si>
 </sst>
 </file>
 
@@ -245,12 +245,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -265,10 +271,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +920,7 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -925,505 +932,513 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>-0.93022324968693937</v>
-      </c>
-      <c r="C2">
-        <v>1.215193166803985E-2</v>
-      </c>
-      <c r="D2">
-        <v>-1.1445352435795604</v>
+      <c r="B3" s="3">
+        <v>5.3815799999999996</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6.0432839999999999</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6.2526840000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>-0.61560961133423886</v>
-      </c>
-      <c r="C3">
-        <v>5.7274733742540995E-2</v>
-      </c>
-      <c r="D3">
-        <v>-0.99268300986137969</v>
+      <c r="B4" s="3">
+        <v>4.3054199999999989</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.0410799999999991</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.2460999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.4151232475852602</v>
-      </c>
-      <c r="C4">
-        <v>1.4087353285558413</v>
-      </c>
-      <c r="D4">
-        <v>0.36506381923858111</v>
+      <c r="B5" s="3">
+        <v>4.4018999999999995</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.9365599999999992</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4.9606799999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1.5756091234656404</v>
-      </c>
-      <c r="C5">
-        <v>2.8778649415214614</v>
-      </c>
-      <c r="D5">
-        <v>1.3272166901460807</v>
+      <c r="B6" s="3">
+        <v>4.7556599999999998</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.6400599999999992</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5.7405599999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>4.3147406974467408</v>
-      </c>
-      <c r="C6">
-        <v>7.7189757459614228</v>
-      </c>
-      <c r="D6">
-        <v>4.3064161360094406</v>
+      <c r="B7" s="3">
+        <v>8.9967599999999983</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10.299239999999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>9.0490199999999987</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1.378812659570162</v>
-      </c>
-      <c r="C7">
-        <v>4.2775721087070018</v>
-      </c>
-      <c r="D7">
-        <v>1.3179730026796825</v>
+      <c r="B8" s="3">
+        <v>11.147459999999999</v>
+      </c>
+      <c r="C8" s="3">
+        <v>12.924299999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11.191679999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>-0.81534641598759805</v>
-      </c>
-      <c r="C8">
-        <v>5.0427855867645981</v>
-      </c>
-      <c r="D8">
-        <v>-2.501350576104997</v>
+      <c r="B9" s="3">
+        <v>28.308839999999996</v>
+      </c>
+      <c r="C9" s="3">
+        <v>31.661519999999999</v>
+      </c>
+      <c r="D9" s="3">
+        <v>26.025479999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0.63626227724556195</v>
-      </c>
-      <c r="C9">
-        <v>2.3261316100167218</v>
-      </c>
-      <c r="D9">
-        <v>0.14614664529264232</v>
+      <c r="B10" s="3">
+        <v>9.5354399999999977</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10.882139999999998</v>
+      </c>
+      <c r="D10" s="3">
+        <v>9.6520199999999985</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>-0.81705678843020024</v>
-      </c>
-      <c r="C10">
-        <v>3.4723910720080013</v>
-      </c>
-      <c r="D10">
-        <v>-2.0087405891881964</v>
+      <c r="B11" s="3">
+        <v>28.52994</v>
+      </c>
+      <c r="C11" s="3">
+        <v>32.943899999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>26.596319999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>-0.41328506442565782</v>
-      </c>
-      <c r="C11">
-        <v>1.204626419388001</v>
-      </c>
-      <c r="D11">
-        <v>-0.94823400605863739</v>
+      <c r="B12" s="3">
+        <v>10.874099999999999</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12.791639999999999</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11.203739999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>0.43129782110572101</v>
-      </c>
-      <c r="C12">
-        <v>2.0719357790177799</v>
-      </c>
-      <c r="D12">
-        <v>-4.3468267975796948E-3</v>
+      <c r="B13" s="3">
+        <v>8.6269199999999984</v>
+      </c>
+      <c r="C13" s="3">
+        <v>10.287179999999999</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10.04196</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>-4.8225613178317985</v>
-      </c>
-      <c r="C13">
-        <v>-4.1122356055897189</v>
-      </c>
-      <c r="D13">
-        <v>-5.2118499085481584</v>
+      <c r="B14" s="3">
+        <v>12.687119999999998</v>
+      </c>
+      <c r="C14" s="3">
+        <v>14.291099999999998</v>
+      </c>
+      <c r="D14" s="3">
+        <v>13.229819999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>-0.78457285750233918</v>
-      </c>
-      <c r="C14">
-        <v>0.37435324558511951</v>
-      </c>
-      <c r="D14">
-        <v>-0.67265977880859928</v>
+      <c r="B15" s="3">
+        <v>5.0812799999999996</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5.2822800000000001</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5.4310199999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>-2.6766366384509999</v>
-      </c>
-      <c r="C15">
-        <v>-1.6799192745368989</v>
-      </c>
-      <c r="D15">
-        <v>-2.7253458367740393</v>
+      <c r="B16" s="3">
+        <v>6.9626399999999995</v>
+      </c>
+      <c r="C16" s="3">
+        <v>7.3244399999999992</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.4892599999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>-2.6160095857268786</v>
-      </c>
-      <c r="C16">
-        <v>-0.16288628590231902</v>
-      </c>
-      <c r="D16">
-        <v>-2.3106746144119992</v>
+      <c r="B17" s="3">
+        <v>12.767519999999999</v>
+      </c>
+      <c r="C17" s="3">
+        <v>14.134319999999999</v>
+      </c>
+      <c r="D17" s="3">
+        <v>12.0198</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>-0.26953010724087978</v>
-      </c>
-      <c r="C17">
-        <v>0.87289907603718042</v>
-      </c>
-      <c r="D17">
-        <v>-0.21262536112423991</v>
+      <c r="B18" s="3">
+        <v>4.7596799999999995</v>
+      </c>
+      <c r="C18" s="3">
+        <v>5.0370599999999994</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4.9767599999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>2.1680580161487804</v>
-      </c>
-      <c r="C18">
-        <v>3.1625627183357805</v>
-      </c>
-      <c r="D18">
-        <v>2.1094363638662195</v>
+      <c r="B19" s="3">
+        <v>1.9175399999999998</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2.2391399999999999</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2.1788400000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>2.4543199525887407</v>
-      </c>
-      <c r="C19">
-        <v>3.8316318333875805</v>
-      </c>
-      <c r="D19">
-        <v>2.73489454208964</v>
+      <c r="B20" s="3">
+        <v>2.3516999999999997</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2.8943999999999996</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3.1235399999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>1.2519506267937603</v>
-      </c>
-      <c r="C20">
-        <v>2.2017197352013609</v>
-      </c>
-      <c r="D20">
-        <v>1.1068646042273804</v>
+      <c r="B21" s="3">
+        <v>2.8622399999999995</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3.5255399999999995</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3.4933799999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>4.38452525328906</v>
-      </c>
-      <c r="C21">
-        <v>6.2126712836736395</v>
-      </c>
-      <c r="D21">
-        <v>5.4331808712523406</v>
+      <c r="B22" s="3">
+        <v>1.7030279999999998</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2.054252</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2.5524999999999993</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>12.231723335911829</v>
-      </c>
-      <c r="C22">
-        <v>16.450966008137581</v>
-      </c>
-      <c r="D22">
-        <v>12.157393093484998</v>
+      <c r="B23" s="3">
+        <v>4.9879253333333313</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5.8304363671738217</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5.8369344348547996</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>5.31084033153076</v>
-      </c>
-      <c r="C23">
-        <v>7.4221166855421998</v>
-      </c>
-      <c r="D23">
-        <v>5.3978097327696606</v>
+      <c r="B24" s="3">
+        <v>2.5157439999999998</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2.9568159999999994</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3.0997559999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>1.0255391856827618</v>
-      </c>
-      <c r="C24">
-        <v>4.0708791590717581</v>
-      </c>
-      <c r="D24">
-        <v>0.78911820937815769</v>
+      <c r="B25" s="3">
+        <v>10.293391999999999</v>
+      </c>
+      <c r="C25" s="3">
+        <v>11.387920000000001</v>
+      </c>
+      <c r="D25" s="3">
+        <v>10.019760000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>0.71411292282116001</v>
-      </c>
-      <c r="C25">
-        <v>1.9128185721453201</v>
-      </c>
-      <c r="D25">
-        <v>-0.36366954573106014</v>
+      <c r="B26" s="3">
+        <v>6.7768800000000002</v>
+      </c>
+      <c r="C26" s="3">
+        <v>7.8703200000000004</v>
+      </c>
+      <c r="D26" s="3">
+        <v>8.7026400000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>-1.8696359398310598</v>
-      </c>
-      <c r="C26">
-        <v>-2.3145580245779609</v>
-      </c>
-      <c r="D26">
-        <v>-2.8858691448029408</v>
+      <c r="B27" s="3">
+        <v>7.9485440000000001</v>
+      </c>
+      <c r="C27" s="3">
+        <v>9.2108640000000008</v>
+      </c>
+      <c r="D27" s="3">
+        <v>9.601776000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>0.68670733101247983</v>
-      </c>
-      <c r="C27">
-        <v>2.2010794406949401</v>
-      </c>
-      <c r="D27">
-        <v>0.66892574423892093</v>
+      <c r="B28" s="3">
+        <v>7.3323599999999995</v>
+      </c>
+      <c r="C28" s="3">
+        <v>8.3798399999999997</v>
+      </c>
+      <c r="D28" s="3">
+        <v>8.3148799999999987</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>-0.50302888173013915</v>
-      </c>
-      <c r="C28">
-        <v>0.13897026276562041</v>
-      </c>
-      <c r="D28">
-        <v>-0.64070382273283943</v>
+      <c r="B29" s="3">
+        <v>4.5350199999999994</v>
+      </c>
+      <c r="C29" s="3">
+        <v>5.24552</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5.2739399999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>1.8194899650067002</v>
-      </c>
-      <c r="C29">
-        <v>3.5343121668098005</v>
-      </c>
-      <c r="D29">
-        <v>2.1494225251725005</v>
+      <c r="B30" s="3">
+        <v>4.1493199999999995</v>
+      </c>
+      <c r="C30" s="3">
+        <v>4.5147199999999996</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4.8313999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>13.891107133251001</v>
-      </c>
-      <c r="C30">
-        <v>20.705081937561598</v>
-      </c>
-      <c r="D30">
-        <v>15.286757076054197</v>
+      <c r="B31" s="3">
+        <v>4.6583679999999994</v>
+      </c>
+      <c r="C31" s="3">
+        <v>5.134792</v>
+      </c>
+      <c r="D31" s="3">
+        <v>5.2528800000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>9.2735642825384197</v>
-      </c>
-      <c r="C31">
-        <v>14.501667973284579</v>
-      </c>
-      <c r="D31">
-        <v>10.463271474530259</v>
+      <c r="B32" s="3">
+        <v>3.8439679999999998</v>
+      </c>
+      <c r="C32" s="3">
+        <v>4.3651840000000002</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4.4384800000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>14.159388634991959</v>
-      </c>
-      <c r="C32">
-        <v>21.024468786748798</v>
-      </c>
-      <c r="D32">
-        <v>12.708938598335358</v>
+      <c r="B33" s="3">
+        <v>4.5402800000000001</v>
+      </c>
+      <c r="C33" s="3">
+        <v>5.2691680000000005</v>
+      </c>
+      <c r="D33" s="3">
+        <v>4.8782559999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>1.3567119012748003</v>
-      </c>
-      <c r="C33">
-        <v>2.9419825641356008</v>
-      </c>
-      <c r="D33">
-        <v>1.6910620639080811</v>
+      <c r="B34" s="3">
+        <v>4.5868199999999995</v>
+      </c>
+      <c r="C34" s="3">
+        <v>4.9646999999999997</v>
+      </c>
+      <c r="D34" s="3">
+        <v>5.1335399999999991</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>-1.0022344031486194</v>
-      </c>
-      <c r="C34">
-        <v>-0.22047123060290019</v>
-      </c>
-      <c r="D34">
-        <v>-1.0648878996748197</v>
+      <c r="B35" s="3">
+        <v>4.3335599999999994</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4.8441000000000001</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4.8280199999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>-0.91504591932221935</v>
-      </c>
-      <c r="C35">
-        <v>-5.2751368822459455E-2</v>
-      </c>
-      <c r="D35">
-        <v>-0.94556591056009953</v>
+      <c r="B36" s="3">
+        <v>4.4742599999999992</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4.6430999999999996</v>
+      </c>
+      <c r="D36" s="3">
+        <v>4.8842999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -1442,38 +1457,38 @@
       <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1">
         <v>1882.5466780847623</v>
@@ -1482,12 +1497,12 @@
         <v>662.97016195992751</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1">
         <v>1074.3473219082637</v>
@@ -1496,12 +1511,12 @@
         <v>378.34930007226421</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1">
         <v>708.94095138182922</v>
@@ -1510,12 +1525,12 @@
         <v>249.66536172999702</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1">
         <v>296.59466497368675</v>
@@ -1524,12 +1539,12 @@
         <v>26.206445143483386</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1">
         <v>269.09396483271786</v>
@@ -1538,12 +1553,12 @@
         <v>23.776544424548927</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1">
         <v>209.42894352843248</v>
@@ -1552,12 +1567,12 @@
         <v>18.504675802319184</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1">
         <v>135.052476318608</v>
@@ -1566,12 +1581,12 @@
         <v>11.932936529553505</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1">
         <v>120.70921180147687</v>
@@ -1580,12 +1595,12 @@
         <v>10.665597567876576</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1">
         <v>37.752215846279597</v>
@@ -1594,12 +1609,12 @@
         <v>13.295071482326987</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
         <v>36.743212274677497</v>
@@ -1608,12 +1623,12 @@
         <v>12.939734072067527</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1">
         <v>32.477930649252315</v>
@@ -1622,12 +1637,12 @@
         <v>11.437644119700611</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1">
         <v>29.272453324927131</v>
@@ -1636,12 +1651,12 @@
         <v>10.308781900449409</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1">
         <v>29.272453324927131</v>
@@ -1650,12 +1665,12 @@
         <v>10.308781900449409</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1">
         <v>581.37437922853599</v>
@@ -1664,12 +1679,12 @@
         <v>60.883155325045131</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1">
         <v>320.81198433622006</v>
@@ -1678,12 +1693,12 @@
         <v>33.596330643941329</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1">
         <v>329.69488987534078</v>
@@ -1692,12 +1707,12 @@
         <v>34.526573422086521</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1">
         <v>204.07809775247023</v>
@@ -1706,12 +1721,12 @@
         <v>12.839331545385168</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1">
         <v>183.16576427104681</v>
@@ -1720,12 +1735,12 @@
         <v>11.523656880084618</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1">
         <v>145.06798226974158</v>
@@ -1734,12 +1749,12 @@
         <v>9.1267800978839926</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1">
         <v>114.57369937173523</v>
@@ -1748,12 +1763,12 @@
         <v>7.2082684463242002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C22" s="1">
         <v>104.58854751596581</v>
@@ -1762,12 +1777,12 @@
         <v>6.5800644566793114</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1">
         <v>52.67839237671604</v>
@@ -1776,12 +1791,12 @@
         <v>5.5166289742612262</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1">
         <v>53.635717158427816</v>
@@ -1790,12 +1805,12 @@
         <v>5.6168827100017236</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1">
         <v>51.142687140136921</v>
@@ -1804,12 +1819,12 @@
         <v>5.3558056153505689</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1">
         <v>40.897041716640437</v>
@@ -1818,12 +1833,12 @@
         <v>4.282852895019448</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1">
         <v>67.786506141750834</v>
@@ -1832,12 +1847,12 @@
         <v>7.098793015004901</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1">
         <v>833.403589493342</v>
@@ -1846,12 +1861,12 @@
         <v>535.79661369384769</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
         <v>511.52097491876253</v>
@@ -1860,12 +1875,12 @@
         <v>330.91047254678278</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1">
         <v>396.74979164146157</v>
@@ -1874,12 +1889,12 @@
         <v>258.05923829854601</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1">
         <v>25.127846695992258</v>
@@ -1888,12 +1903,12 @@
         <v>12.352611651086642</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1">
         <v>20.372060899175683</v>
@@ -1902,12 +1917,12 @@
         <v>9.2253555858477156</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C33" s="1">
         <v>15.631128039930639</v>
@@ -1916,12 +1931,12 @@
         <v>6.8239221975646558</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1">
         <v>16.188110155319194</v>
@@ -1930,12 +1945,12 @@
         <v>6.3340868359932632</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1">
         <v>16.083205524600658</v>
@@ -1944,12 +1959,12 @@
         <v>6.3828653528090094</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C36" s="1">
         <v>5.1920011400039741</v>
@@ -1958,12 +1973,12 @@
         <v>2.4669983568493095</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1">
         <v>4.366953108768338</v>
@@ -1972,12 +1987,12 @@
         <v>1.8587443245012361</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1">
         <v>5.2050197936378941</v>
@@ -1986,12 +2001,12 @@
         <v>2.4327329815864416</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C39" s="1">
         <v>2.735459785711468</v>
@@ -2000,12 +2015,12 @@
         <v>1.3451893143186251</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1">
         <v>1.8274781876488513</v>
@@ -2027,40 +2042,40 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
         <v>1882.5466780847623</v>
@@ -2069,18 +2084,18 @@
         <v>662.97016195992751</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1">
         <v>1074.3473219082637</v>
@@ -2089,18 +2104,18 @@
         <v>378.34930007226421</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1">
         <v>708.94095138182922</v>
@@ -2109,18 +2124,18 @@
         <v>249.66536172999702</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <v>296.59466497368675</v>
@@ -2129,18 +2144,18 @@
         <v>26.206445143483386</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1">
         <v>269.09396483271786</v>
@@ -2149,18 +2164,18 @@
         <v>23.776544424548927</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1">
         <v>209.42894352843248</v>
@@ -2169,18 +2184,18 @@
         <v>18.504675802319184</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1">
         <v>135.052476318608</v>
@@ -2189,18 +2204,18 @@
         <v>11.932936529553505</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1">
         <v>120.70921180147687</v>
@@ -2209,18 +2224,18 @@
         <v>10.665597567876576</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1">
         <v>37.752215846279597</v>
@@ -2229,18 +2244,18 @@
         <v>13.295071482326987</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1">
         <v>36.743212274677497</v>
@@ -2249,18 +2264,18 @@
         <v>12.939734072067527</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1">
         <v>32.477930649252315</v>
@@ -2269,18 +2284,18 @@
         <v>11.437644119700611</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1">
         <v>29.272453324927131</v>
@@ -2289,18 +2304,18 @@
         <v>10.308781900449409</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1">
         <v>29.272453324927131</v>
@@ -2309,185 +2324,185 @@
         <v>10.308781900449409</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2503,41 +2518,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB065429-5795-4F63-8637-68CB66573FC8}">
   <dimension ref="A1:XFD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -18916,15 +18931,15 @@
       <c r="XFC1" s="2"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1">
         <v>833.403589493342</v>
@@ -18941,18 +18956,18 @@
         <v>878.98135502803041</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1">
         <v>511.52097491876253</v>
@@ -18969,18 +18984,18 @@
         <v>501.42248670819981</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1">
         <v>396.74979164146157</v>
@@ -18997,18 +19012,18 @@
         <v>468.38544321825634</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1">
         <v>25.127846695992258</v>
@@ -19025,18 +19040,18 @@
         <v>216.85333279737583</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1">
         <v>20.372060899175683</v>
@@ -19053,18 +19068,18 @@
         <v>194.31246958437478</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
         <v>15.631128039930639</v>
@@ -19081,18 +19096,18 @@
         <v>153.87518811210757</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1">
         <v>16.188110155319194</v>
@@ -19109,18 +19124,18 @@
         <v>124.42772269106116</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1">
         <v>16.083205524600658</v>
@@ -19137,18 +19152,18 @@
         <v>114.28888768775747</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1">
         <v>5.1920011400039741</v>
@@ -19165,18 +19180,18 @@
         <v>55.403395159870705</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1">
         <v>4.366953108768338</v>
@@ -19193,18 +19208,18 @@
         <v>56.143925942694914</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1">
         <v>5.2050197936378941</v>
@@ -19221,18 +19236,18 @@
         <v>53.914973952188376</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1">
         <v>2.735459785711468</v>
@@ -19249,18 +19264,18 @@
         <v>42.287312188033283</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1">
         <v>1.8274781876488513</v>
@@ -19277,18 +19292,18 @@
         <v>68.819527160796213</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1">
         <v>581.37437922853599</v>
@@ -19305,18 +19320,18 @@
         <v>520.49122390349089</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1">
         <v>320.81198433622006</v>
@@ -19333,18 +19348,18 @@
         <v>287.21565369227875</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>329.69488987534078</v>
@@ -19361,18 +19376,18 @@
         <v>295.16831645325425</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1">
         <v>204.07809775247023</v>
@@ -19389,18 +19404,18 @@
         <v>191.23876620708506</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1">
         <v>183.16576427104681</v>
@@ -19417,18 +19432,18 @@
         <v>171.6421073909622</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1">
         <v>145.06798226974158</v>
@@ -19445,18 +19460,18 @@
         <v>135.94120217185758</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1">
         <v>114.57369937173523</v>
@@ -19473,18 +19488,18 @@
         <v>107.36543092541103</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1">
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1">
         <v>104.58854751596581</v>
@@ -19501,18 +19516,18 @@
         <v>98.008483059286505</v>
       </c>
       <c r="H22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1">
         <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D23" s="1">
         <v>52.67839237671604</v>
@@ -19529,18 +19544,18 @@
         <v>47.161763402454817</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1">
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1">
         <v>53.635717158427816</v>
@@ -19557,18 +19572,18 @@
         <v>48.018834448426091</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1">
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1">
         <v>51.142687140136921</v>
@@ -19585,18 +19600,18 @@
         <v>45.786881524786352</v>
       </c>
       <c r="H25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1">
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D26" s="1">
         <v>40.897041716640437</v>
@@ -19613,18 +19628,18 @@
         <v>36.614188821620992</v>
       </c>
       <c r="H26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1">
         <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D27" s="1">
         <v>67.786506141750834</v>
@@ -19641,7 +19656,7 @@
         <v>60.687713126745933</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>